<commit_message>
added signal to noise and conservation score
</commit_message>
<xml_diff>
--- a/data/KCNQ1/1. Raw/KCNQ1_concise_Updated GnomAD.xlsx
+++ b/data/KCNQ1/1. Raw/KCNQ1_concise_Updated GnomAD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python\gene-VUS-prediction\data\KCNQ1\1. Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767A0112-BD74-4CCE-8963-78E7FA1F0562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD0733D-E766-4142-94A6-178613E3B446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" firstSheet="2" activeTab="4" xr2:uid="{ABBA9FBB-02E7-CA49-A142-658C5C2DF7EC}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="2" activeTab="4" xr2:uid="{ABBA9FBB-02E7-CA49-A142-658C5C2DF7EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Benign_Likely Benign" sheetId="1" r:id="rId1"/>
@@ -10388,7 +10388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CF7569-8A6D-884C-A27F-6C9BDE3B3298}">
   <dimension ref="A1:C690"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A603" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>